<commit_message>
setup electron and switch to neon db
</commit_message>
<xml_diff>
--- a/imports/employee-import-template.xlsx
+++ b/imports/employee-import-template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="179">
   <si>
     <t xml:space="preserve">first_name</t>
   </si>
@@ -170,7 +170,7 @@
     <t xml:space="preserve">HR Manager</t>
   </si>
   <si>
-    <t xml:space="preserve">GameCove</t>
+    <t xml:space="preserve">GC</t>
   </si>
   <si>
     <t xml:space="preserve">Regular</t>
@@ -344,7 +344,7 @@
     <t xml:space="preserve">Sales &amp; Ops Assistant</t>
   </si>
   <si>
-    <t xml:space="preserve">Luxium</t>
+    <t xml:space="preserve">LX</t>
   </si>
   <si>
     <t xml:space="preserve">05/28/2025</t>
@@ -557,13 +557,7 @@
     <t xml:space="preserve">Job Title</t>
   </si>
   <si>
-    <t xml:space="preserve">GC</t>
-  </si>
-  <si>
     <t xml:space="preserve">GameCove Inc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LX</t>
   </si>
   <si>
     <t xml:space="preserve">Luxium Trading Inc.</t>
@@ -859,8 +853,8 @@
   </sheetPr>
   <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA7" activeCellId="0" sqref="AA7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA8" activeCellId="0" sqref="AA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1617,7 +1611,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AA7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AA8 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1976,7 +1970,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AA7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AA8 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2044,7 +2038,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="AA7 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="AA8 A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2111,7 +2105,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AA7 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AA8 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2130,18 +2124,18 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>179</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add penalties and fixed tax withlding + custom overwrite pay per employee
</commit_message>
<xml_diff>
--- a/imports/employee-import-template.xlsx
+++ b/imports/employee-import-template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="200">
   <si>
     <t xml:space="preserve">first_name</t>
   </si>
@@ -384,6 +384,69 @@
   </si>
   <si>
     <t xml:space="preserve">10/27/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Orlando JR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Figueroa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Del Prado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1999/05/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jayrdelprado@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1920 visayan st. Cor mindanao sampaloc manila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sampaloc, Manila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rowena Del Prado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">767-179-156-000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">907-372-035-1324</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/09/2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noemi Stephanie </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capundan </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clidoro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2001/02/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clidorostephanienoemi593@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1028 F.Viscaya St.brgy 194 tondo manila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jess Vicent A. Seguero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Live in Partner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">509-374-631-00000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02/10/2026</t>
   </si>
   <si>
     <t xml:space="preserve">Field</t>
@@ -567,9 +630,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -637,7 +701,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -660,6 +724,18 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -851,10 +927,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG8"/>
+  <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA8" activeCellId="0" sqref="AA8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X11" activeCellId="0" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1583,6 +1659,176 @@
         <v>51</v>
       </c>
     </row>
+    <row r="9" customFormat="false" ht="50.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="K9" s="6" t="n">
+        <v>9270784701</v>
+      </c>
+      <c r="L9" s="6" t="n">
+        <v>9270784701</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="R9" s="6" t="n">
+        <v>639542630492</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="T9" s="6" t="n">
+        <v>3469619408</v>
+      </c>
+      <c r="U9" s="6" t="n">
+        <v>2053108503</v>
+      </c>
+      <c r="V9" s="6" t="n">
+        <v>121205892210</v>
+      </c>
+      <c r="W9" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="X9" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y9" s="6" t="n">
+        <v>9270784701</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC9" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="K10" s="6" t="n">
+        <v>9351309521</v>
+      </c>
+      <c r="L10" s="6" t="n">
+        <v>9351309521</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="R10" s="6" t="n">
+        <v>9650925880</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="6" t="n">
+        <v>9650925880</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC10" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" display="delmundobrixter1636@gmail.com"/>
@@ -1592,6 +1838,8 @@
     <hyperlink ref="I6" r:id="rId5" display="xtianmayquez@gmail.com"/>
     <hyperlink ref="I7" r:id="rId6" display="kenzzmercado@gmail.com"/>
     <hyperlink ref="I8" r:id="rId7" display="ggylianfae@gmail.com"/>
+    <hyperlink ref="I9" r:id="rId8" display="jayrdelprado@gmail.com"/>
+    <hyperlink ref="I10" r:id="rId9" display="clidorostephanienoemi593@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1611,7 +1859,7 @@
   <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AA8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1622,39 +1870,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1662,7 +1910,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,7 +1918,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,7 +1926,7 @@
         <v>27</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1686,13 +1934,13 @@
         <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1700,7 +1948,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,7 +1956,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1716,7 +1964,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,7 +1972,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,7 +1980,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,7 +1988,7 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,7 +1996,7 @@
         <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1756,7 +2004,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1764,7 +2012,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,7 +2020,7 @@
         <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,7 +2028,7 @@
         <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1788,7 +2036,7 @@
         <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1796,7 +2044,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,13 +2052,13 @@
         <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,7 +2066,7 @@
         <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1826,7 +2074,7 @@
         <v>17</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1834,13 +2082,13 @@
         <v>18</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1848,7 +2096,7 @@
         <v>19</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1856,7 +2104,7 @@
         <v>20</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1864,7 +2112,7 @@
         <v>21</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,13 +2120,13 @@
         <v>22</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1886,7 +2134,7 @@
         <v>23</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1894,13 +2142,13 @@
         <v>24</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,7 +2156,7 @@
         <v>25</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,7 +2164,7 @@
         <v>26</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,7 +2172,7 @@
         <v>29</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1932,7 +2180,7 @@
         <v>30</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1940,7 +2188,7 @@
         <v>31</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1948,7 +2196,7 @@
         <v>32</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -1970,7 +2218,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AA8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1981,42 +2229,42 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2038,7 +2286,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="AA8 A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2048,7 +2296,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2105,7 +2353,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AA8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2116,10 +2364,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2127,7 +2375,7 @@
         <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2135,7 +2383,7 @@
         <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>